<commit_message>
Implemented best time and best score in the menu
</commit_message>
<xml_diff>
--- a/files/quiz_data.xlsx
+++ b/files/quiz_data.xlsx
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>999999</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>999999</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Added total score and time in the menus
</commit_message>
<xml_diff>
--- a/files/quiz_data.xlsx
+++ b/files/quiz_data.xlsx
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>21</v>
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>17</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>999999</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Got misc quiz data and fixed list menu
</commit_message>
<xml_diff>
--- a/files/quiz_data.xlsx
+++ b/files/quiz_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwwgi\Documents\Coding stuff\esc_app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB710AE-36F9-4330-B7D9-AAB8BD6E3E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E691C1-8664-4958-AA5C-F43AA5031FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,7 +577,7 @@
   <dimension ref="A1:D125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,6 +2305,9 @@
       <c r="B123" s="1">
         <v>0</v>
       </c>
+      <c r="C123" s="1">
+        <v>1758</v>
+      </c>
       <c r="D123" s="1">
         <v>999999</v>
       </c>
@@ -2331,7 +2334,7 @@
         <v>0</v>
       </c>
       <c r="C125" s="1">
-        <v>1758</v>
+        <v>91</v>
       </c>
       <c r="D125" s="1">
         <v>999999</v>

</xml_diff>

<commit_message>
Merging for year column in all entries quiz
</commit_message>
<xml_diff>
--- a/files/quiz_data.xlsx
+++ b/files/quiz_data.xlsx
@@ -2293,13 +2293,13 @@
         </is>
       </c>
       <c r="B123" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C123" s="1" t="n">
         <v>1758</v>
       </c>
       <c r="D123" s="1" t="n">
-        <v>999999</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124">

</xml_diff>

<commit_message>
Debugging quizzes_list_menu data updating
</commit_message>
<xml_diff>
--- a/files/quiz_data.xlsx
+++ b/files/quiz_data.xlsx
@@ -1325,13 +1325,13 @@
         <v>1956</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>14</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>999999</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55">
@@ -1339,13 +1339,13 @@
         <v>1957</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>999999</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56">
@@ -1353,13 +1353,13 @@
         <v>1958</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>999999</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57">

</xml_diff>

<commit_message>
quizzes_list_menu displayed data updating fixed
</commit_message>
<xml_diff>
--- a/files/quiz_data.xlsx
+++ b/files/quiz_data.xlsx
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>17</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -1325,13 +1325,13 @@
         <v>1956</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>14</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>13</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55">
@@ -1451,13 +1451,13 @@
         <v>1965</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>18</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>999999</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64">

</xml_diff>

<commit_message>
Adjusting data display size when updating data
</commit_message>
<xml_diff>
--- a/files/quiz_data.xlsx
+++ b/files/quiz_data.xlsx
@@ -1493,13 +1493,13 @@
         <v>1968</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>17</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>999999</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67">

</xml_diff>